<commit_message>
IA-17 Fix invoice generation: filter by client_id and exclude HIREUP shifts
- Add client_id filter to ensure only shifts for the selected client are included
- Exclude shifts with category='HIREUP' from invoices
- Add validation to require clientId parameter
</commit_message>
<xml_diff>
--- a/Invoice_template.xlsx
+++ b/Invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrozhogin/invoice_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120314C5-8AD5-7D4D-92DC-C70745184358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19F541F-D5F5-914E-8B26-093C369C40C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="800" windowWidth="36760" windowHeight="23940" xr2:uid="{EBC12D85-38C0-DA49-8B3F-00F65F1D33ED}"/>
   </bookViews>
@@ -409,6 +409,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -420,9 +423,6 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,7 +750,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="4" max="5" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="24.1640625" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
@@ -935,7 +935,7 @@
       <c r="B16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -944,20 +944,20 @@
       <c r="E16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="20"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="21"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="18" t="s">
         <v>6</v>
       </c>
@@ -974,20 +974,20 @@
       <c r="E17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="14" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="23"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="16" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Add invoice history tracking and Invoices page
Features:
- Create invoices table to store generated invoice metadata
- Add save-invoice API endpoint to record generated invoices
- Add list-invoices API endpoint to retrieve all invoices with carer/client details
- Add delete-invoice API endpoint to remove invoice records
- Add download-invoice API endpoint to regenerate and download invoices
- Create Invoices page with:
  - Instructions on how to generate invoices from Calendar
  - Table showing: Invoice#, Carer, Client, DateFrom, DateTo, InvoiceDate, Generated timestamp
  - Download button to retrieve invoice files
  - Delete button to remove invoice records
  - Sorted by generation date (newest first)
- Update generate-invoice endpoint to save invoice record after generation
- Add Invoices link to main navigation menu
- Update Supabase types to include Invoice table
</commit_message>
<xml_diff>
--- a/Invoice_template.xlsx
+++ b/Invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrozhogin/invoice_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19F541F-D5F5-914E-8B26-093C369C40C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F6C1EE-6D3D-1142-86A9-2BFF10F29676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="800" windowWidth="36760" windowHeight="23940" xr2:uid="{EBC12D85-38C0-DA49-8B3F-00F65F1D33ED}"/>
   </bookViews>
@@ -406,9 +406,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,6 +420,9 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,7 +744,7 @@
   <dimension ref="B2:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,10 +932,10 @@
     </row>
     <row r="15" spans="2:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -944,20 +944,20 @@
       <c r="E16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="21"/>
       <c r="L16" s="18" t="s">
         <v>6</v>
       </c>
@@ -974,20 +974,20 @@
       <c r="E17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="14" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="24"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="16" t="s">
         <v>36</v>
       </c>

</xml_diff>